<commit_message>
Add ExcelUtility and update step definitions to handle Excel data
Introduced ExcelUtility for reading and writing Excel files. Modified step definitions to utilize Excel data for creating and deleting citizenship entries. Updated Hooks to log test results in Excel.
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resource/ApacheExcel2.xlsx
+++ b/src/test/java/ApachePOI/resource/ApacheExcel2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TechnoStudy\IdeaProjects\Cucumber7\src\test\java\ApachePOI\resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yasemin Monster\IdeaProjects\Cucumber\src\test\java\ApachePOI\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AC8E1949-3393-423E-90A9-C0078393D53A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="17280" windowHeight="8970" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,30 +64,6 @@
     <t>bes</t>
   </si>
   <si>
-    <t>ulais1145</t>
-  </si>
-  <si>
-    <t>ulais1146</t>
-  </si>
-  <si>
-    <t>ulais1147</t>
-  </si>
-  <si>
-    <t>ulais1148</t>
-  </si>
-  <si>
-    <t>ulais1149</t>
-  </si>
-  <si>
-    <t>ulais1150</t>
-  </si>
-  <si>
-    <t>ulais1151</t>
-  </si>
-  <si>
-    <t>ulais1152</t>
-  </si>
-  <si>
     <t>urbs13</t>
   </si>
   <si>
@@ -109,12 +86,36 @@
   </si>
   <si>
     <t>urbs20</t>
+  </si>
+  <si>
+    <t>yulais1145</t>
+  </si>
+  <si>
+    <t>yulais1146</t>
+  </si>
+  <si>
+    <t>uylais1147</t>
+  </si>
+  <si>
+    <t>uylais1148</t>
+  </si>
+  <si>
+    <t>ulais1y151</t>
+  </si>
+  <si>
+    <t>ulaisy1150</t>
+  </si>
+  <si>
+    <t>ulayis1149</t>
+  </si>
+  <si>
+    <t>ulyais1152</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -426,16 +427,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -443,7 +444,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -457,7 +458,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -465,7 +466,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -473,7 +474,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -481,7 +482,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -489,7 +490,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -497,7 +498,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -509,25 +510,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
       <c r="C1" t="s">
         <v>8</v>
       </c>
@@ -541,13 +542,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
@@ -561,13 +562,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
@@ -581,13 +582,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
@@ -601,53 +602,53 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>24</v>
       </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
@@ -661,12 +662,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
         <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>

</xml_diff>